<commit_message>
More work and part tracking
</commit_message>
<xml_diff>
--- a/MouserBOM.xlsx
+++ b/MouserBOM.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10211"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10311"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kevinhardin/Documents/EAGLE/projects/Dual Mono Amp Design/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kevinhardin/Documents/EAGLE/projects/Dual-Mono-Amp-Design/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75F9E3DB-410B-F04D-91E1-5BC983DECE0A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE581544-9EFA-7843-A27E-D5DE38D73438}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="23500" xr2:uid="{5705E612-2462-F143-B726-090DE75A8E16}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="217" uniqueCount="147">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="218" uniqueCount="147">
   <si>
     <t>Value</t>
   </si>
@@ -2662,8 +2662,8 @@
           </cell>
         </row>
       </sheetData>
-      <sheetData sheetId="1" refreshError="1"/>
-      <sheetData sheetId="2" refreshError="1"/>
+      <sheetData sheetId="1"/>
+      <sheetData sheetId="2"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -2968,8 +2968,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6623A4E5-CFAC-CE4C-A34F-C1D14525D2DA}">
   <dimension ref="A1:S21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O30" sqref="O30"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="I18" sqref="I18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4101,6 +4101,9 @@
       <c r="H18" t="s">
         <v>66</v>
       </c>
+      <c r="I18" t="s">
+        <v>66</v>
+      </c>
       <c r="J18" t="s">
         <v>66</v>
       </c>

</xml_diff>

<commit_message>
Added AK4493 breakout boards
</commit_message>
<xml_diff>
--- a/MouserBOM.xlsx
+++ b/MouserBOM.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10311"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11207"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kevinhardin/Documents/EAGLE/projects/Dual-Mono-Amp-Design/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE581544-9EFA-7843-A27E-D5DE38D73438}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59E83355-6038-4749-B998-0E794B347CAC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="23500" xr2:uid="{5705E612-2462-F143-B726-090DE75A8E16}"/>
   </bookViews>
@@ -2968,7 +2968,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6623A4E5-CFAC-CE4C-A34F-C1D14525D2DA}">
   <dimension ref="A1:S21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="I18" sqref="I18"/>
     </sheetView>
   </sheetViews>

</xml_diff>